<commit_message>
added a test for question file import
</commit_message>
<xml_diff>
--- a/question101.xlsx
+++ b/question101.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="C4" authorId="0">
@@ -63,26 +63,32 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
+    <font>
+      <sz val="10"/>
+      <name val="나눔고딕"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -147,16 +153,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -177,15 +191,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -222,6 +236,8 @@
         <f aca="false">B3/A3</f>
         <v>2.33333333333333</v>
       </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -234,6 +250,8 @@
         <f aca="false">B4/A4</f>
         <v>2</v>
       </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -259,13 +277,54 @@
         <v>1.83333333333333</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="3"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D17" s="2"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,보통"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,보통"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>